<commit_message>
Updated and renamed data for city-owned properties and scavenger tax sale data; added 2019 tax year tax sale data for ward 20
</commit_message>
<xml_diff>
--- a/city-owned-map/data/scavenger-sale/property_classes.xlsx
+++ b/city-owned-map/data/scavenger-sale/property_classes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claire/Documents/programming/editable-map/city-owned-map/data/scavenger-sale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DB6EDA-AD2D-2A4F-95E4-40C9DBAC23DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71423983-0C12-EF4F-9A1A-FDEE7D8B849F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27360" windowHeight="17040" xr2:uid="{A17A7707-86BB-5A44-82C2-6772E814C77E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="tmpdata" localSheetId="0">Sheet1!$A$2:$B$199</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,8 +36,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{FCF8B43E-B816-D34E-A18D-1FF53EBDE0FE}" name="tmpdata" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/claire/Downloads/tmpdata.txt">
+      <textFields count="2">
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="351">
   <si>
     <t>property_code</t>
   </si>
@@ -75,15 +91,9 @@
     <t>Apartment building with 2 to 6 units, any age</t>
   </si>
   <si>
-    <t>Residential land</t>
-  </si>
-  <si>
     <t>First-time agricultural use of land valued at market price</t>
   </si>
   <si>
-    <t>Vacant land under common ownership with adjacent</t>
-  </si>
-  <si>
     <t>Residential garage</t>
   </si>
   <si>
@@ -237,9 +247,6 @@
     <t>Quonset hut or butler type building</t>
   </si>
   <si>
-    <t>Golf course improvement</t>
-  </si>
-  <si>
     <t>Commercial minor improvement</t>
   </si>
   <si>
@@ -1081,14 +1088,37 @@
   </si>
   <si>
     <t>Unclassified</t>
+  </si>
+  <si>
+    <t>2-18</t>
+  </si>
+  <si>
+    <t>A residential building licensed as a Bed &amp; Breakfast by the municipality, County of Cook or registered as a Bed &amp; Breakfast with the State of Illinois under 50 ILCS 820/1 et.seq., with six or fewer rentable units and where one unit is owner occupied and is entitled to a Homeowner‚Äôs Exemption pursuant to the Property Tax Code.</t>
+  </si>
+  <si>
+    <t>2-19</t>
+  </si>
+  <si>
+    <t>A residential building licensed as a Bed &amp; Breakfast by the municipality, County of Cook or registered as a Bed &amp; Breakfast with the State of Illinois under 50 ILCS 820/1 et.seq., with six or fewer rentable units and where none of the units is owner occupied and no Homeowner‚Äôs Exemption is allowed pursuant to the Property Tax Code.</t>
+  </si>
+  <si>
+    <t>Vacant land under common ownership with adjacent residence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1116,10 +1146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,6 +1167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tmpdata" connectionId="1" xr16:uid="{274FB888-87BE-224D-BE34-4201B17C2DC8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1433,2238 +1469,2206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DC8B44-3655-9A4C-B26D-A09F21DAC1F8}">
-  <dimension ref="A1:C202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E005526-F5AA-D646-A5A4-3D7D2CEAC701}">
+  <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C1" t="s">
-        <v>346</v>
+      <c r="B1" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B2" t="s">
-        <v>348</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>344</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
+        <v>155</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
+        <v>156</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" t="s">
-        <v>111</v>
+        <v>157</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
+        <v>158</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
+        <v>159</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" t="s">
-        <v>114</v>
+        <v>162</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" t="s">
-        <v>115</v>
+        <v>163</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
+        <v>164</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
+        <v>165</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
+        <v>169</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" t="s">
-        <v>118</v>
+        <v>170</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
+        <v>346</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
+        <v>348</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
+        <v>166</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
+        <v>171</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
+        <v>172</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
+        <v>173</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B30" t="s">
-        <v>119</v>
+        <v>167</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B31" t="s">
-        <v>20</v>
+        <v>168</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
+        <v>174</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B33" t="s">
-        <v>120</v>
+        <v>175</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
+        <v>176</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B35" t="s">
-        <v>23</v>
+        <v>177</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
+        <v>178</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
+        <v>179</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B38" t="s">
-        <v>121</v>
+        <v>180</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B39" t="s">
-        <v>122</v>
+        <v>181</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B40" t="s">
-        <v>123</v>
+        <v>182</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B41" t="s">
-        <v>26</v>
+        <v>183</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B42" t="s">
-        <v>27</v>
+        <v>184</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B43" t="s">
-        <v>124</v>
+        <v>185</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B44" t="s">
-        <v>28</v>
+        <v>186</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
+        <v>187</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
+        <v>188</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B47" t="s">
-        <v>31</v>
+        <v>189</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B48" t="s">
-        <v>125</v>
+        <v>190</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" t="s">
-        <v>126</v>
+        <v>191</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B50" t="s">
-        <v>32</v>
+        <v>192</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B51" t="s">
-        <v>33</v>
+        <v>193</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
+        <v>194</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B53" t="s">
-        <v>35</v>
+        <v>195</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" t="s">
-        <v>36</v>
+        <v>196</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B55" t="s">
-        <v>37</v>
+        <v>197</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B56" t="s">
-        <v>38</v>
+        <v>198</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B57" t="s">
-        <v>39</v>
+        <v>199</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B58" t="s">
-        <v>40</v>
+        <v>200</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
+        <v>201</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B60" t="s">
-        <v>42</v>
+        <v>202</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B61" t="s">
-        <v>43</v>
+        <v>203</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B62" t="s">
-        <v>127</v>
+        <v>204</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B63" t="s">
-        <v>44</v>
+        <v>205</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C63" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B64" t="s">
-        <v>45</v>
+        <v>206</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B65" t="s">
-        <v>46</v>
+        <v>207</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B66" t="s">
-        <v>47</v>
+        <v>208</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B67" t="s">
-        <v>48</v>
+        <v>209</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B68" t="s">
-        <v>128</v>
+        <v>210</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B69" t="s">
-        <v>49</v>
+        <v>211</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B70" t="s">
-        <v>129</v>
+        <v>212</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C70" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B71" t="s">
-        <v>50</v>
+        <v>213</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B72" t="s">
-        <v>51</v>
+        <v>214</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B73" t="s">
-        <v>52</v>
+        <v>215</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B74" t="s">
-        <v>53</v>
+        <v>216</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B75" t="s">
-        <v>54</v>
+        <v>217</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B76" t="s">
-        <v>55</v>
+        <v>218</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B77" t="s">
-        <v>56</v>
+        <v>219</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C77" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B78" t="s">
-        <v>57</v>
+        <v>220</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B79" t="s">
-        <v>58</v>
+        <v>221</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C79" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B80" t="s">
-        <v>59</v>
+        <v>222</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C80" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B81" t="s">
-        <v>60</v>
+        <v>223</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B82" t="s">
-        <v>61</v>
+        <v>224</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C82" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B83" t="s">
-        <v>62</v>
+        <v>225</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B84" t="s">
-        <v>63</v>
+        <v>226</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B85" t="s">
-        <v>64</v>
+        <v>227</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C85" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B86" t="s">
-        <v>65</v>
+        <v>228</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B87" t="s">
-        <v>66</v>
+        <v>229</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C87" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B88" t="s">
-        <v>67</v>
+        <v>230</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C88" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B89" t="s">
-        <v>68</v>
+        <v>231</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C89" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B90" t="s">
-        <v>69</v>
+        <v>232</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C90" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B91" t="s">
-        <v>130</v>
+        <v>233</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C91" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B92" t="s">
-        <v>70</v>
+        <v>234</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C92" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B93" t="s">
-        <v>71</v>
+        <v>235</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B94" t="s">
-        <v>72</v>
+        <v>236</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B95" t="s">
-        <v>73</v>
+        <v>237</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B96" t="s">
-        <v>74</v>
+        <v>238</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C96" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B97" t="s">
-        <v>75</v>
+        <v>239</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B98" t="s">
-        <v>76</v>
+        <v>240</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C98" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B99" t="s">
-        <v>77</v>
+        <v>241</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B100" t="s">
-        <v>78</v>
+        <v>242</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C100" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B101" t="s">
-        <v>72</v>
+        <v>243</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C101" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B102" t="s">
-        <v>73</v>
+        <v>244</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C102" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B103" t="s">
-        <v>131</v>
+        <v>245</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C103" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B104" t="s">
-        <v>75</v>
+        <v>246</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C104" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B105" t="s">
-        <v>76</v>
+        <v>247</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C105" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B106" t="s">
-        <v>77</v>
+        <v>248</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C106" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B107" t="s">
-        <v>78</v>
+        <v>249</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C107" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B108" t="s">
-        <v>72</v>
+        <v>250</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B109" t="s">
-        <v>78</v>
+        <v>251</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C109" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B110" t="s">
-        <v>73</v>
+        <v>252</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C110" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B111" t="s">
-        <v>131</v>
+        <v>253</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C111" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B112" t="s">
-        <v>75</v>
+        <v>254</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C112" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B113" t="s">
-        <v>76</v>
+        <v>255</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C113" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B114" t="s">
-        <v>77</v>
+        <v>256</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C114" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B115" t="s">
-        <v>79</v>
+        <v>257</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C115" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B116" t="s">
-        <v>80</v>
+        <v>258</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C116" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B117" t="s">
-        <v>81</v>
+        <v>259</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C117" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B118" t="s">
-        <v>132</v>
+        <v>260</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="C118" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B119" t="s">
-        <v>82</v>
+        <v>261</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C119" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B120" t="s">
-        <v>83</v>
+        <v>262</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C120" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B121" t="s">
-        <v>84</v>
+        <v>263</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C121" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B122" t="s">
-        <v>85</v>
+        <v>264</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C122" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B123" t="s">
-        <v>86</v>
+        <v>265</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C123" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B124" t="s">
-        <v>133</v>
+        <v>266</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="C124" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B125" t="s">
-        <v>87</v>
+        <v>267</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C125" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B126" t="s">
-        <v>88</v>
+        <v>268</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="C126" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B127" t="s">
-        <v>89</v>
+        <v>269</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C127" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B128" t="s">
-        <v>90</v>
+        <v>270</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C128" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B129" t="s">
-        <v>59</v>
+        <v>271</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B130" t="s">
-        <v>60</v>
+        <v>272</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C130" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B131" t="s">
-        <v>61</v>
+        <v>273</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C131" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B132" t="s">
-        <v>62</v>
+        <v>274</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C132" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B133" t="s">
-        <v>63</v>
+        <v>275</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C133" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B134" t="s">
-        <v>64</v>
+        <v>276</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C134" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B135" t="s">
-        <v>65</v>
+        <v>277</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C135" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B136" t="s">
-        <v>66</v>
+        <v>278</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C136" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B137" t="s">
-        <v>67</v>
+        <v>279</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="C137" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B138" t="s">
-        <v>91</v>
+        <v>280</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="C138" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B139" t="s">
-        <v>92</v>
+        <v>281</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C139" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B140" t="s">
-        <v>130</v>
+        <v>282</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C140" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B141" t="s">
-        <v>70</v>
+        <v>283</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C141" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B142" t="s">
-        <v>93</v>
+        <v>284</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="C142" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B143" t="s">
-        <v>94</v>
+        <v>285</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C143" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B144" t="s">
-        <v>53</v>
+        <v>286</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C144" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B145" t="s">
-        <v>134</v>
+        <v>287</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C145" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B146" t="s">
-        <v>67</v>
+      <c r="B146" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C146" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B147" t="s">
-        <v>87</v>
+        <v>289</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C147" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B148" t="s">
-        <v>56</v>
+        <v>290</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C148" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B149" t="s">
-        <v>62</v>
+        <v>291</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C149" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B150" t="s">
-        <v>89</v>
+        <v>292</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C150" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B151" t="s">
-        <v>95</v>
+        <v>293</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C151" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B152" t="s">
+        <v>294</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C152" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B153" t="s">
-        <v>60</v>
+        <v>295</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C153" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B154" t="s">
-        <v>61</v>
+        <v>296</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="C154" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B155" t="s">
+        <v>297</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C155" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B156" t="s">
-        <v>135</v>
+        <v>298</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C156" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B157" t="s">
-        <v>65</v>
+        <v>299</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C157" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B158" t="s">
-        <v>66</v>
+        <v>300</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C158" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B159" t="s">
-        <v>96</v>
+        <v>301</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="C159" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B160" t="s">
-        <v>70</v>
+        <v>302</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C160" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B161" t="s">
-        <v>136</v>
+        <v>303</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C161" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B162" t="s">
-        <v>97</v>
+        <v>304</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="C162" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B163" t="s">
-        <v>98</v>
+        <v>305</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C163" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B164" t="s">
-        <v>94</v>
+        <v>306</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C164" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B165" t="s">
-        <v>53</v>
+        <v>307</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C165" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B166" t="s">
-        <v>99</v>
+        <v>308</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C166" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B167" t="s">
-        <v>134</v>
+        <v>309</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C167" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B168" t="s">
-        <v>55</v>
+        <v>310</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C168" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B169" t="s">
-        <v>56</v>
+        <v>311</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C169" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B170" t="s">
-        <v>89</v>
+        <v>312</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C170" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B171" t="s">
-        <v>100</v>
+        <v>313</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C171" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B172" t="s">
+        <v>314</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C172" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B173" t="s">
+        <v>315</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C173" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B174" t="s">
+        <v>316</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C174" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B175" t="s">
-        <v>62</v>
+        <v>317</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="C175" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B176" t="s">
+        <v>318</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C176" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B177" t="s">
-        <v>135</v>
+        <v>319</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C177" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B178" t="s">
-        <v>65</v>
+        <v>320</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C178" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B179" t="s">
-        <v>66</v>
+        <v>321</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C179" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B180" t="s">
-        <v>67</v>
+        <v>322</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C180" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C181" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B182" t="s">
-        <v>131</v>
+      <c r="B182" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C182" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B183" t="s">
-        <v>66</v>
+      <c r="B183" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="C183" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B184" t="s">
-        <v>76</v>
+      <c r="B184" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C184" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B185" t="s">
-        <v>77</v>
+      <c r="B185" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C185" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B186" t="s">
-        <v>101</v>
+      <c r="B186" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C186" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B187" t="s">
-        <v>97</v>
+      <c r="B187" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C187" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B188" t="s">
-        <v>130</v>
+      <c r="B188" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="C188" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B189" t="s">
-        <v>78</v>
+      <c r="B189" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C189" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B190" t="s">
-        <v>70</v>
+      <c r="B190" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C190" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C191" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B192" t="s">
-        <v>103</v>
+      <c r="B192" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="C192" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B193" t="s">
-        <v>104</v>
+      <c r="B193" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="C193" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B194" t="s">
-        <v>105</v>
+      <c r="B194" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C194" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B195" t="s">
-        <v>137</v>
+      <c r="B195" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C195" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B196" t="s">
-        <v>138</v>
+      <c r="B196" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="C196" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B197" t="s">
-        <v>139</v>
+      <c r="B197" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C197" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B198" t="s">
-        <v>106</v>
+      <c r="B198" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C198" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B199" t="s">
-        <v>107</v>
+      <c r="B199" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C199" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B200" t="s">
-        <v>108</v>
-      </c>
-      <c r="C200" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="B201" t="s">
-        <v>124</v>
-      </c>
-      <c r="C201" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B202" t="s">
-        <v>28</v>
-      </c>
-      <c r="C202" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>